<commit_message>
Update TLTK.xlsx with new data and adjustments
</commit_message>
<xml_diff>
--- a/public/TLTK/TLTK.xlsx
+++ b/public/TLTK/TLTK.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="144">
   <si>
     <t>        'QC-FSH': 'fas fa-broom',            // Quality Control/Fresh - Vệ sinh</t>
   </si>
@@ -408,12 +408,6 @@
     <t>Chỉnh sửa RE task</t>
   </si>
   <si>
-    <t>Button Hủy</t>
-  </si>
-  <si>
-    <t>Button Cập nhật</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -421,6 +415,48 @@
   </si>
   <si>
     <t>Xác nhận đồng ý thay đổi thông tin</t>
+  </si>
+  <si>
+    <t>Select Task Position</t>
+  </si>
+  <si>
+    <t>Check box</t>
+  </si>
+  <si>
+    <t>Select Task Position Linked</t>
+  </si>
+  <si>
+    <t>Hủy</t>
+  </si>
+  <si>
+    <t>Cập nhật</t>
+  </si>
+  <si>
+    <t>Xác nhận</t>
+  </si>
+  <si>
+    <t>List Postion</t>
+  </si>
+  <si>
+    <t>Task khác</t>
+  </si>
+  <si>
+    <t>Task giống với vị trí chính</t>
+  </si>
+  <si>
+    <t>Button 2 trạng thái</t>
+  </si>
+  <si>
+    <t>List Task</t>
+  </si>
+  <si>
+    <t>Mỗi dòng tương ứng với list position</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -476,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -485,6 +521,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,20 +586,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>394872</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>183968</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -570,8 +612,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="7448550"/>
-          <a:ext cx="4052472" cy="3562350"/>
+          <a:off x="5019674" y="7448550"/>
+          <a:ext cx="3638551" cy="3784418"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -582,20 +624,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>156898</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>968212</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -608,8 +650,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295774" y="7439025"/>
-          <a:ext cx="3438525" cy="3576373"/>
+          <a:off x="8753475" y="7467600"/>
+          <a:ext cx="3216112" cy="3848100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -620,20 +662,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>942974</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>159096</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>160119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="6" name="Picture 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -646,8 +688,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7953375" y="7439025"/>
-          <a:ext cx="2990849" cy="3578571"/>
+          <a:off x="0" y="7439025"/>
+          <a:ext cx="4876800" cy="4722594"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1169,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="P1:AA102"/>
+  <dimension ref="P1:AA106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1225,7 @@
     <col min="19" max="19" width="29.85546875" customWidth="1"/>
     <col min="20" max="20" width="35.7109375" customWidth="1"/>
     <col min="21" max="21" width="15" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="16:21" x14ac:dyDescent="0.25">
@@ -1690,42 +1732,174 @@
     </row>
     <row r="57" spans="19:23" x14ac:dyDescent="0.25">
       <c r="T57" t="s">
+        <v>133</v>
+      </c>
+      <c r="U57" t="s">
         <v>127</v>
       </c>
-      <c r="U57" t="s">
-        <v>129</v>
-      </c>
       <c r="W57" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="19:23" x14ac:dyDescent="0.25">
       <c r="T58" t="s">
+        <v>134</v>
+      </c>
+      <c r="U58" t="s">
+        <v>127</v>
+      </c>
+      <c r="W58" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T59" t="s">
+        <v>143</v>
+      </c>
+      <c r="U59" t="s">
+        <v>127</v>
+      </c>
+      <c r="W59" t="s">
         <v>128</v>
       </c>
-      <c r="U58" t="s">
+    </row>
+    <row r="61" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="S61" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T63" t="s">
+        <v>136</v>
+      </c>
+      <c r="U63" t="s">
+        <v>131</v>
+      </c>
+      <c r="V63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="S64" s="3"/>
+      <c r="T64" t="s">
+        <v>135</v>
+      </c>
+      <c r="U64" t="s">
+        <v>127</v>
+      </c>
+      <c r="W64" t="s">
         <v>129</v>
       </c>
-      <c r="W58" t="s">
+    </row>
+    <row r="65" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="S65" s="3"/>
+      <c r="T65" t="s">
+        <v>143</v>
+      </c>
+      <c r="U65" t="s">
+        <v>127</v>
+      </c>
+      <c r="W65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="S66" s="3"/>
+    </row>
+    <row r="67" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="S67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="V68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T69" t="s">
+        <v>136</v>
+      </c>
+      <c r="U69" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="60" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S60" s="3"/>
-    </row>
-    <row r="63" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S63" s="3"/>
-    </row>
-    <row r="72" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S72" s="3"/>
+      <c r="V69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T70" t="s">
+        <v>137</v>
+      </c>
+      <c r="U70" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="V70" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="W70" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T71" t="s">
+        <v>138</v>
+      </c>
+      <c r="U71" s="6"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="6"/>
+    </row>
+    <row r="72" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T72" t="s">
+        <v>140</v>
+      </c>
+      <c r="U72" t="s">
+        <v>114</v>
+      </c>
+      <c r="V72" t="s">
+        <v>117</v>
+      </c>
+      <c r="W72" s="6"/>
+    </row>
+    <row r="73" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T73" t="s">
+        <v>135</v>
+      </c>
+      <c r="U73" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T74" t="s">
+        <v>143</v>
+      </c>
+      <c r="U74" t="s">
+        <v>127</v>
+      </c>
+      <c r="W74" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="S75" s="3"/>
     </row>
     <row r="101" spans="23:27" x14ac:dyDescent="0.25">
       <c r="AA101" s="1"/>
     </row>
-    <row r="102" spans="23:27" x14ac:dyDescent="0.25">
-      <c r="W102" s="2"/>
+    <row r="106" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W106" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="U70:U71"/>
+    <mergeCell ref="W70:W72"/>
+    <mergeCell ref="V70:V71"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Timeframe selection popup and enhance Position selection functionality
</commit_message>
<xml_diff>
--- a/public/TLTK/TLTK.xlsx
+++ b/public/TLTK/TLTK.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="136">
   <si>
     <t>        'QC-FSH': 'fas fa-broom',            // Quality Control/Fresh - Vệ sinh</t>
   </si>
@@ -291,9 +291,6 @@
     <t>1 (Cố định), CTM, …</t>
   </si>
   <si>
-    <t>= Frequency_Coeff x Frequency_Count x RE_Unit x Store_Parameter</t>
-  </si>
-  <si>
     <t>nếu cố định thì =1, nếu biến động thì lấy tham số cửa hàng tương ứng</t>
   </si>
   <si>
@@ -342,30 +339,15 @@
     <t>Xoá task</t>
   </si>
   <si>
-    <t>Sự kiện</t>
-  </si>
-  <si>
     <t>Edit Task</t>
   </si>
   <si>
     <t>Delete Task</t>
   </si>
   <si>
-    <t>Vị trí</t>
-  </si>
-  <si>
-    <t>Trong bảng, cuối mỗi dòng quản lý task</t>
-  </si>
-  <si>
-    <t>Logic</t>
-  </si>
-  <si>
     <t>Popup</t>
   </si>
   <si>
-    <t>Click =&gt; Open Confirm Popup "Xác nhận xoá task"</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -381,33 +363,12 @@
     <t>String</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Lấy tại Screen Quản lý nhóm task</t>
-  </si>
-  <si>
-    <t>Lấy từ database</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Input (Disable)</t>
   </si>
   <si>
-    <t>Tính toán bằng công thức</t>
-  </si>
-  <si>
     <t>Task Position Linked</t>
   </si>
   <si>
-    <t>Click =&gt; Open Popup "Chỉnh sửa RE task"</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa RE task</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -429,9 +390,6 @@
     <t>Hủy</t>
   </si>
   <si>
-    <t>Cập nhật</t>
-  </si>
-  <si>
     <t>Xác nhận</t>
   </si>
   <si>
@@ -453,10 +411,28 @@
     <t>Mỗi dòng tương ứng với list position</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa RE task/Thêm mới RE Task</t>
+  </si>
+  <si>
+    <t>Cập nhật/Thêm mới</t>
+  </si>
+  <si>
+    <t>Xác nhận đồng ý thay đổi thông tin/Xác nhận thêm mới Task</t>
+  </si>
+  <si>
+    <t>= Frequency_Coeff x Frequency_Count x RE_Unit x Store_Parameter / 60</t>
+  </si>
+  <si>
+    <t>Người dùng lựa chọn</t>
+  </si>
+  <si>
+    <t>App tự tính toán</t>
+  </si>
+  <si>
+    <t>Người dùng nhập vào</t>
   </si>
 </sst>
 </file>
@@ -512,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -523,9 +499,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,13 +561,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>183968</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -612,7 +585,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5019674" y="7448550"/>
+          <a:off x="5019674" y="6686550"/>
           <a:ext cx="3638551" cy="3784418"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -626,13 +599,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>968212</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -650,7 +623,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8753475" y="7467600"/>
+          <a:off x="8753475" y="6705600"/>
           <a:ext cx="3216112" cy="3848100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -664,13 +637,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>160119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -688,7 +661,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="7439025"/>
+          <a:off x="0" y="6677025"/>
           <a:ext cx="4876800" cy="4722594"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1211,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="P1:AA106"/>
+  <dimension ref="P1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,6 +1199,7 @@
     <col min="20" max="20" width="35.7109375" customWidth="1"/>
     <col min="21" max="21" width="15" customWidth="1"/>
     <col min="22" max="22" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="16:21" x14ac:dyDescent="0.25">
@@ -1267,7 +1241,7 @@
     </row>
     <row r="10" spans="16:21" x14ac:dyDescent="0.25">
       <c r="R10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="16:21" x14ac:dyDescent="0.25">
@@ -1280,35 +1254,35 @@
     </row>
     <row r="12" spans="16:21" x14ac:dyDescent="0.25">
       <c r="S12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="T12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="U12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="16:21" x14ac:dyDescent="0.25">
       <c r="S13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="16:21" x14ac:dyDescent="0.25">
       <c r="S14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="U14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="16:21" x14ac:dyDescent="0.25">
@@ -1363,7 +1337,7 @@
         <v>87</v>
       </c>
       <c r="U19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="19:21" x14ac:dyDescent="0.25">
@@ -1379,7 +1353,7 @@
     </row>
     <row r="21" spans="19:21" x14ac:dyDescent="0.25">
       <c r="U21" s="5" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="19:21" x14ac:dyDescent="0.25">
@@ -1395,48 +1369,48 @@
     </row>
     <row r="23" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T23" t="s">
         <v>60</v>
       </c>
       <c r="U23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S24" t="s">
+        <v>94</v>
+      </c>
+      <c r="U24" t="s">
         <v>95</v>
-      </c>
-      <c r="U24" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="19:21" x14ac:dyDescent="0.25">
       <c r="T25" t="s">
+        <v>96</v>
+      </c>
+      <c r="U25" t="s">
         <v>97</v>
-      </c>
-      <c r="U25" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="26" spans="19:21" x14ac:dyDescent="0.25">
       <c r="T26" t="s">
+        <v>98</v>
+      </c>
+      <c r="U26" t="s">
         <v>99</v>
-      </c>
-      <c r="U26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="27" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S27" t="s">
+        <v>89</v>
+      </c>
+      <c r="T27" t="s">
         <v>90</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>91</v>
-      </c>
-      <c r="U27" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="28" spans="19:21" x14ac:dyDescent="0.25">
@@ -1474,431 +1448,391 @@
     </row>
     <row r="31" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S31" t="s">
+        <v>101</v>
+      </c>
+      <c r="T31" t="s">
+        <v>104</v>
+      </c>
+      <c r="U31" t="s">
         <v>102</v>
-      </c>
-      <c r="T31" t="s">
-        <v>106</v>
-      </c>
-      <c r="U31" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="32" spans="19:21" x14ac:dyDescent="0.25">
       <c r="T32" t="s">
+        <v>105</v>
+      </c>
+      <c r="U32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="R34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="S36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="U37" t="s">
         <v>107</v>
       </c>
-      <c r="U32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="R33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T34" t="s">
+      <c r="V37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T38" t="s">
+        <v>48</v>
+      </c>
+      <c r="U38" t="s">
         <v>108</v>
       </c>
-      <c r="U34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="S35" t="s">
+      <c r="V38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T39" t="s">
+        <v>50</v>
+      </c>
+      <c r="U39" t="s">
+        <v>108</v>
+      </c>
+      <c r="V39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T40" t="s">
+        <v>49</v>
+      </c>
+      <c r="U40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T41" t="s">
+        <v>51</v>
+      </c>
+      <c r="U41" t="s">
+        <v>108</v>
+      </c>
+      <c r="V41" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T42" t="s">
+        <v>80</v>
+      </c>
+      <c r="U42" t="s">
+        <v>112</v>
+      </c>
+      <c r="V42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T43" t="s">
+        <v>67</v>
+      </c>
+      <c r="U43" t="s">
+        <v>109</v>
+      </c>
+      <c r="V43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T44" t="s">
+        <v>58</v>
+      </c>
+      <c r="U44" t="s">
+        <v>109</v>
+      </c>
+      <c r="V44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T45" t="s">
+        <v>86</v>
+      </c>
+      <c r="U45" t="s">
+        <v>108</v>
+      </c>
+      <c r="V45" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T46" t="s">
+        <v>83</v>
+      </c>
+      <c r="U46" t="s">
+        <v>112</v>
+      </c>
+      <c r="V46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T47" t="s">
+        <v>77</v>
+      </c>
+      <c r="U47" t="s">
         <v>106</v>
       </c>
-      <c r="T35" t="s">
+      <c r="V47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="T48" t="s">
+        <v>113</v>
+      </c>
+      <c r="U48" t="s">
+        <v>106</v>
+      </c>
+      <c r="V48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U49" t="s">
+        <v>106</v>
+      </c>
+      <c r="V49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T50" t="s">
+        <v>61</v>
+      </c>
+      <c r="U50" t="s">
         <v>109</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T51" t="s">
+        <v>63</v>
+      </c>
+      <c r="U51" t="s">
+        <v>109</v>
+      </c>
+      <c r="V51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T52" t="s">
+        <v>66</v>
+      </c>
+      <c r="U52" t="s">
+        <v>109</v>
+      </c>
+      <c r="V52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T53" t="s">
+        <v>120</v>
+      </c>
+      <c r="U53" t="s">
+        <v>114</v>
+      </c>
+      <c r="V53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T54" t="s">
+        <v>130</v>
+      </c>
+      <c r="U54" t="s">
+        <v>114</v>
+      </c>
+      <c r="V54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T55" t="s">
+        <v>128</v>
+      </c>
+      <c r="U55" t="s">
+        <v>114</v>
+      </c>
+      <c r="V55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="T59" t="s">
+        <v>122</v>
+      </c>
+      <c r="U59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S60" s="3"/>
+      <c r="T60" t="s">
+        <v>121</v>
+      </c>
+      <c r="U60" t="s">
+        <v>114</v>
+      </c>
+      <c r="V60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S61" s="3"/>
+      <c r="T61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U61" t="s">
+        <v>114</v>
+      </c>
+      <c r="V61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S62" s="3"/>
+    </row>
+    <row r="63" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T65" t="s">
+        <v>122</v>
+      </c>
+      <c r="U65" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T66" t="s">
+        <v>123</v>
+      </c>
+      <c r="U66" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="36" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="S36" t="s">
-        <v>107</v>
-      </c>
-      <c r="T36" t="s">
-        <v>109</v>
-      </c>
-      <c r="U36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="R38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="S40" t="s">
+      <c r="V66" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T67" t="s">
+        <v>124</v>
+      </c>
+      <c r="U67" s="6"/>
+      <c r="V67" s="6"/>
+    </row>
+    <row r="68" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T68" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="41" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="U41" t="s">
-        <v>113</v>
-      </c>
-      <c r="V41" t="s">
-        <v>116</v>
-      </c>
-      <c r="W41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T42" t="s">
-        <v>48</v>
-      </c>
-      <c r="U42" t="s">
-        <v>114</v>
-      </c>
-      <c r="V42" t="s">
-        <v>117</v>
-      </c>
-      <c r="W42" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T43" t="s">
-        <v>50</v>
-      </c>
-      <c r="U43" t="s">
-        <v>114</v>
-      </c>
-      <c r="V43" t="s">
-        <v>117</v>
-      </c>
-      <c r="W43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T44" t="s">
-        <v>49</v>
-      </c>
-      <c r="U44" t="s">
-        <v>115</v>
-      </c>
-      <c r="V44" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T45" t="s">
-        <v>51</v>
-      </c>
-      <c r="U45" t="s">
-        <v>114</v>
-      </c>
-      <c r="V45" t="s">
-        <v>117</v>
-      </c>
-      <c r="W45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T46" t="s">
-        <v>80</v>
-      </c>
-      <c r="U46" t="s">
-        <v>122</v>
-      </c>
-      <c r="V46" t="s">
-        <v>121</v>
-      </c>
-      <c r="W46" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T47" t="s">
-        <v>67</v>
-      </c>
-      <c r="U47" t="s">
-        <v>115</v>
-      </c>
-      <c r="V47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="18:23" x14ac:dyDescent="0.25">
-      <c r="T48" t="s">
-        <v>58</v>
-      </c>
-      <c r="U48" t="s">
-        <v>115</v>
-      </c>
-      <c r="V48" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T49" t="s">
-        <v>86</v>
-      </c>
-      <c r="U49" t="s">
-        <v>114</v>
-      </c>
-      <c r="V49" t="s">
-        <v>117</v>
-      </c>
-      <c r="W49" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T50" t="s">
-        <v>83</v>
-      </c>
-      <c r="U50" t="s">
-        <v>122</v>
-      </c>
-      <c r="V50" t="s">
-        <v>121</v>
-      </c>
-      <c r="W50" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T51" t="s">
-        <v>77</v>
-      </c>
-      <c r="U51" t="s">
-        <v>111</v>
-      </c>
-      <c r="W51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T52" t="s">
-        <v>124</v>
-      </c>
-      <c r="U52" t="s">
-        <v>111</v>
-      </c>
-      <c r="W52" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T53" t="s">
-        <v>90</v>
-      </c>
-      <c r="U53" t="s">
-        <v>115</v>
-      </c>
-      <c r="V53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T54" t="s">
-        <v>61</v>
-      </c>
-      <c r="U54" t="s">
-        <v>115</v>
-      </c>
-      <c r="V54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T55" t="s">
-        <v>63</v>
-      </c>
-      <c r="U55" t="s">
-        <v>115</v>
-      </c>
-      <c r="V55" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T56" t="s">
-        <v>66</v>
-      </c>
-      <c r="U56" t="s">
-        <v>115</v>
-      </c>
-      <c r="V56" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T57" t="s">
-        <v>133</v>
-      </c>
-      <c r="U57" t="s">
-        <v>127</v>
-      </c>
-      <c r="W57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T58" t="s">
-        <v>134</v>
-      </c>
-      <c r="U58" t="s">
-        <v>127</v>
-      </c>
-      <c r="W58" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T59" t="s">
-        <v>143</v>
-      </c>
-      <c r="U59" t="s">
-        <v>127</v>
-      </c>
-      <c r="W59" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="61" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="V62" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="63" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T63" t="s">
-        <v>136</v>
-      </c>
-      <c r="U63" t="s">
-        <v>131</v>
-      </c>
-      <c r="V63" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S64" s="3"/>
-      <c r="T64" t="s">
-        <v>135</v>
-      </c>
-      <c r="U64" t="s">
-        <v>127</v>
-      </c>
-      <c r="W64" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S65" s="3"/>
-      <c r="T65" t="s">
-        <v>143</v>
-      </c>
-      <c r="U65" t="s">
-        <v>127</v>
-      </c>
-      <c r="W65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S66" s="3"/>
-    </row>
-    <row r="67" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S67" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="68" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="V68" t="s">
-        <v>116</v>
-      </c>
+      <c r="U68" t="s">
+        <v>108</v>
+      </c>
+      <c r="V68" s="6"/>
     </row>
     <row r="69" spans="19:23" x14ac:dyDescent="0.25">
       <c r="T69" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="U69" t="s">
-        <v>131</v>
-      </c>
-      <c r="V69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="19:23" x14ac:dyDescent="0.25">
       <c r="T70" t="s">
-        <v>137</v>
-      </c>
-      <c r="U70" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="V70" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="W70" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
+      </c>
+      <c r="U70" t="s">
+        <v>114</v>
+      </c>
+      <c r="V70" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T71" t="s">
-        <v>138</v>
-      </c>
-      <c r="U71" s="6"/>
-      <c r="V71" s="7"/>
-      <c r="W71" s="6"/>
+      <c r="S71" s="3"/>
     </row>
     <row r="72" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T72" t="s">
-        <v>140</v>
-      </c>
-      <c r="U72" t="s">
-        <v>114</v>
-      </c>
-      <c r="V72" t="s">
-        <v>117</v>
-      </c>
-      <c r="W72" s="6"/>
+      <c r="S72" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="73" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="T73" t="s">
-        <v>135</v>
-      </c>
-      <c r="U73" t="s">
-        <v>127</v>
+      <c r="V73" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="19:23" x14ac:dyDescent="0.25">
       <c r="T74" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="U74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W74" t="s">
+        <v>118</v>
+      </c>
+      <c r="V74" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T75" t="s">
+        <v>121</v>
+      </c>
+      <c r="U75" t="s">
+        <v>114</v>
+      </c>
+      <c r="W75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="19:23" x14ac:dyDescent="0.25">
+      <c r="T76" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="75" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S75" s="3"/>
+      <c r="U76" t="s">
+        <v>114</v>
+      </c>
+      <c r="W76" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="101" spans="23:27" x14ac:dyDescent="0.25">
       <c r="AA101" s="1"/>
     </row>
-    <row r="106" spans="23:27" x14ac:dyDescent="0.25">
-      <c r="W106" s="2"/>
+    <row r="102" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W102" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="U70:U71"/>
-    <mergeCell ref="W70:W72"/>
-    <mergeCell ref="V70:V71"/>
+  <mergeCells count="2">
+    <mergeCell ref="U66:U67"/>
+    <mergeCell ref="V66:V68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>